<commit_message>
Requirements.txt and new venv
</commit_message>
<xml_diff>
--- a/results/data/10_25_2022/19_30_53_robothor.xlsx
+++ b/results/data/10_25_2022/19_30_53_robothor.xlsx
@@ -540,37 +540,37 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[81, 92]</t>
+          <t>[81, 92, 96]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[0.342, 0.368]</t>
+          <t>[0.342, 0.368, 0.383]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[0, 30]</t>
+          <t>[0, 30, 60]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[0, 19.2872091293335]</t>
+          <t>[0, 19.2872091293335, 32.3680762052536]</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[0, 12.77]</t>
+          <t>[0, 12.77, 23.91]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, 0, -10, 0, -10, -10, -10, -20, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, -20, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, -20, -10, -20, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, -10, -10, -10, 0, 0, 0, -10, 0, 0, 0, 0, 0, 0, -20]</t>
+          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, 0, -10, 0, -10, -10, -10, -20, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, -20, -20, -10, -20, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, 0, 0, -10, -10, -10, 0, 0, 0, 0, 0, -10, 0, 0, 0, 0, 0, -20]</t>
         </is>
       </c>
     </row>
@@ -609,37 +609,37 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[81, 83]</t>
+          <t>[81, 83, 87]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[0.342, 0.352]</t>
+          <t>[0.342, 0.352, 0.372]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[0, 30]</t>
+          <t>[0, 30, 60]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[0, 21.07679290771486]</t>
+          <t>[0, 21.07679290771486, 35.30058748722078]</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>[0, 5.49]</t>
+          <t>[0, 5.49, 12.61]</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, -20, 0, 0, -10, 0, 0, -10, -10, 0, -10, 0, -20, -10, 0, 0, 0, -20, -10, -10, 0, -20, -20, 0, -20, 0, -20, -20, 0, 0, 0, -10, 0, 0, -10, -10, -20, 0, 0, -10, -20, -10, -10, -10, 0, -20, 0, 0, -20, 0, 0, -10, -20, 0, -10, -20, 0, 0, -20, 0, -10, 0, 0, 0, -20, -10, 0, -10, 0, -20, 0, -10, -20, -20, 0, -20, 0, 0]</t>
+          <t>[0, -20, -10, 0, -20, -20, -10, 0, 0, 0, -20, -10, 0, -20, -20, -20, 0, 0, -10, 0, 0, -20, 0, -10, -10, -10, -10, -10, -20, 0, 0, -10, 0, 0, -10, 0, -10, 0, -10, -20, 0, -20, 0, 0, 0, -20, -10, 0, 0, 0, 0, -20, -20, 0, -20, -10, -10, 0, 0, 0, -10, -20, 0, 0, 0, -20, 0, 0, -10, 0, -20, 0, 0, 0, -10, 0, 0, 0, -20, -10, -20]</t>
         </is>
       </c>
     </row>
@@ -678,32 +678,32 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1']</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[81, 86]</t>
+          <t>[81, 86, 88]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[0.342, 0.367]</t>
+          <t>[0.342, 0.367, 0.382]</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[0, 30]</t>
+          <t>[0, 30, 60]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>[0, 21.99642496109011]</t>
+          <t>[0, 21.99642496109011, 40.14257609844209]</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>[0, 8.27]</t>
+          <t>[0, 8.27, 16.81]</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">

</xml_diff>